<commit_message>
deduplicate and group sources
</commit_message>
<xml_diff>
--- a/tests/repos/original_sheets/Other Coder_Lang [NOCODE_lang].xlsx
+++ b/tests/repos/original_sheets/Other Coder_Lang [NOCODE_lang].xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t xml:space="preserve">Grambank ID</t>
   </si>
@@ -49,9 +49,6 @@
     <t xml:space="preserve">There are no articles. Specificity is marked by a derivational suffix.</t>
   </si>
   <si>
-    <t xml:space="preserve">GB021</t>
-  </si>
-  <si>
     <t xml:space="preserve">Do indefinite nominals commonly have indefinite articles?</t>
   </si>
   <si>
@@ -65,21 +62,6 @@
   </si>
   <si>
     <t xml:space="preserve">Arsjo (1999:92-93)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GB023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Are there postnominal articles?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GB172</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Can an article agree with the noun in gender/noun class?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arsjo (1999:92)</t>
   </si>
 </sst>
 </file>
@@ -209,18 +191,18 @@
   <dimension ref="A1:E65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="8:8"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.35714285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="61.4642857142857"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.35714285714286"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="26.6377551020408"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="10.8877551020408"/>
-    <col collapsed="false" hidden="false" max="256" min="6" style="1" width="9.35714285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="9.35714285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.89795918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="65.8775510204082"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.89795918367347"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="28.530612244898"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="256" min="6" style="1" width="9.89795918367347"/>
+    <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="9.89795918367347"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -259,78 +241,50 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="C3" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>11</v>
       </c>
       <c r="E3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>13</v>
       </c>
       <c r="C4" s="4" t="n">
         <v>0</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>14</v>
-      </c>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="3"/>
       <c r="E5" s="4"/>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>19</v>
-      </c>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="3"/>
       <c r="E6" s="4"/>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="4"/>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="4"/>
-    </row>
+    <row r="1048385" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048386" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048387" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048388" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048389" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>